<commit_message>
listanhallinta toimii, salasanalla voi lisata itsensa whitelistille
</commit_message>
<xml_diff>
--- a/WHITELIST.xlsx
+++ b/WHITELIST.xlsx
@@ -348,77 +348,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A16"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>21942357</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>170633010</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1"/>
-    <row r="15" spans="1:1"/>
-    <row r="16" spans="1:1"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>